<commit_message>
Généralisation à la ville - FrInpatientMedicationRequest hérite du profil générique FrMedicationRequest  (#93)
* heritage

* correct error

* add comment

* update MEdicationRequest (rm todispense, ufrole, notescope)

* cleaning

* update

* correct error dbb4057e3b081fe013a46a0d2886bacf48d8c827
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-fr-additional-action-relationship-type.xlsx
+++ b/main/ig/CodeSystem-fr-additional-action-relationship-type.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-31T09:35:58+00:00</t>
+    <t>2025-08-08T09:43:11+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -120,7 +120,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>2</t>
+    <t>1</t>
   </si>
   <si>
     <t>Level</t>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>Definition</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>ALT</t>
@@ -474,13 +471,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="C2" t="s" s="2">
         <v>41</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>42</v>
       </c>
       <c r="D2" s="2"/>
     </row>

</xml_diff>